<commit_message>
Add extra data to Race line excel sheet
</commit_message>
<xml_diff>
--- a/documents/Race line 27 points plus extras to force splines.xlsx
+++ b/documents/Race line 27 points plus extras to force splines.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\sjors\evgp\documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D378FB1D-FA2E-4FD5-AF0B-5CFEA22527C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="468" yWindow="684" windowWidth="8844" windowHeight="8640"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Raceline Data" sheetId="1" r:id="rId1"/>
@@ -34,7 +40,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -183,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -210,17 +216,20 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -231,6 +240,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -279,7 +291,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -312,9 +324,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -347,6 +376,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -522,11 +568,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:K42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -537,45 +583,46 @@
     <col min="5" max="6" width="8.88671875" style="1"/>
     <col min="7" max="7" width="4.77734375" style="6" customWidth="1"/>
     <col min="8" max="9" width="8.88671875" style="1"/>
+    <col min="10" max="10" width="9.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="10" t="s">
+    <row r="2" spans="2:11" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="13"/>
       <c r="D2" s="7"/>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="11"/>
+      <c r="F2" s="13"/>
       <c r="G2" s="8"/>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="11"/>
-    </row>
-    <row r="3" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="12" t="s">
+      <c r="I2" s="13"/>
+    </row>
+    <row r="3" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="11" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" s="2">
         <v>237.12204501344434</v>
       </c>
@@ -595,8 +642,14 @@
       <c r="I4" s="2">
         <v>116.88091083956182</v>
       </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J4" s="14">
+        <v>0</v>
+      </c>
+      <c r="K4" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
         <v>280.44530701738847</v>
       </c>
@@ -616,8 +669,14 @@
       <c r="I5" s="2">
         <v>88.023169527657004</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J5" s="14">
+        <v>1</v>
+      </c>
+      <c r="K5" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" s="2">
         <v>303.79985940175919</v>
       </c>
@@ -637,8 +696,14 @@
       <c r="I6" s="2">
         <v>90.070052563394796</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J6" s="14">
+        <v>2</v>
+      </c>
+      <c r="K6" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" s="2">
         <v>315.24509753798009</v>
       </c>
@@ -658,8 +723,14 @@
       <c r="I7" s="2">
         <v>97.809880823188379</v>
       </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J7" s="14">
+        <v>3</v>
+      </c>
+      <c r="K7" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
         <v>336.74927869877416</v>
       </c>
@@ -679,8 +750,14 @@
       <c r="I8" s="3">
         <v>98.009885962836734</v>
       </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J8" s="14">
+        <v>4</v>
+      </c>
+      <c r="K8" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" s="2">
         <v>348.35532395570038</v>
       </c>
@@ -700,8 +777,14 @@
       <c r="I9" s="2">
         <v>95.470667724155618</v>
       </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J9" s="14">
+        <v>5</v>
+      </c>
+      <c r="K9" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>355.78502035716491</v>
       </c>
@@ -721,8 +804,14 @@
       <c r="I10" s="3">
         <v>91.189385705893542</v>
       </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J10" s="14">
+        <v>6</v>
+      </c>
+      <c r="K10" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" s="2">
         <v>358.49465798436637</v>
       </c>
@@ -742,8 +831,14 @@
       <c r="I11" s="2">
         <v>82.044629044957389</v>
       </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J11" s="14">
+        <v>7</v>
+      </c>
+      <c r="K11" s="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" s="2">
         <v>362.75737304924036</v>
       </c>
@@ -763,8 +858,14 @@
       <c r="I12" s="2">
         <v>34.297151943377621</v>
       </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J12" s="14">
+        <v>8</v>
+      </c>
+      <c r="K12" s="14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <v>359.95653032464594</v>
       </c>
@@ -784,8 +885,14 @@
       <c r="I13" s="3">
         <v>20.736589447790269</v>
       </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J13" s="14">
+        <v>9</v>
+      </c>
+      <c r="K13" s="14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B14" s="2">
         <v>353.66007151365449</v>
       </c>
@@ -805,8 +912,14 @@
       <c r="I14" s="2">
         <v>16.798266932207646</v>
       </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J14" s="14">
+        <v>10</v>
+      </c>
+      <c r="K14" s="14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <v>343.22388445973331</v>
       </c>
@@ -826,8 +939,14 @@
       <c r="I15" s="3">
         <v>16.051651035193242</v>
       </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J15" s="14">
+        <v>11</v>
+      </c>
+      <c r="K15" s="14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B16" s="2">
         <v>323.86721230533198</v>
       </c>
@@ -847,8 +966,14 @@
       <c r="I16" s="2">
         <v>18.945127481098027</v>
       </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J16" s="14">
+        <v>12</v>
+      </c>
+      <c r="K16" s="14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B17" s="2">
         <v>215.70670288130515</v>
       </c>
@@ -868,8 +993,14 @@
       <c r="I17" s="2">
         <v>59.328841755698797</v>
       </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J17" s="14">
+        <v>13</v>
+      </c>
+      <c r="K17" s="14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" s="2">
         <v>130.60045163180851</v>
       </c>
@@ -889,8 +1020,14 @@
       <c r="I18" s="2">
         <v>72.296879529155689</v>
       </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J18" s="14">
+        <v>14</v>
+      </c>
+      <c r="K18" s="14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" s="2">
         <v>60.497884151477422</v>
       </c>
@@ -910,8 +1047,14 @@
       <c r="I19" s="2">
         <v>38.211623808146413</v>
       </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J19" s="14">
+        <v>15</v>
+      </c>
+      <c r="K19" s="14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <v>29.796860303453336</v>
       </c>
@@ -931,8 +1074,14 @@
       <c r="I20" s="3">
         <v>19.06043933615895</v>
       </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J20" s="14">
+        <v>16</v>
+      </c>
+      <c r="K20" s="14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" s="2">
         <v>16.328533797133641</v>
       </c>
@@ -952,8 +1101,14 @@
       <c r="I21" s="2">
         <v>19.888738405443419</v>
       </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J21" s="14">
+        <v>17</v>
+      </c>
+      <c r="K21" s="14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <v>6.9552966136729184</v>
       </c>
@@ -973,8 +1128,14 @@
       <c r="I22" s="3">
         <v>24.88862744747064</v>
       </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J22" s="14">
+        <v>18</v>
+      </c>
+      <c r="K22" s="14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B23" s="2">
         <v>16.853128270908556</v>
       </c>
@@ -994,8 +1155,14 @@
       <c r="I23" s="2">
         <v>47.05943858614129</v>
       </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J23" s="14">
+        <v>19</v>
+      </c>
+      <c r="K23" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B24" s="2">
         <v>80.253673551298604</v>
       </c>
@@ -1015,8 +1182,14 @@
       <c r="I24" s="2">
         <v>119.08379673551539</v>
       </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J24" s="14">
+        <v>20</v>
+      </c>
+      <c r="K24" s="14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B25" s="2">
         <v>96.081829175953487</v>
       </c>
@@ -1036,8 +1209,14 @@
       <c r="I25" s="2">
         <v>146.46535658844729</v>
       </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J25" s="14">
+        <v>21</v>
+      </c>
+      <c r="K25" s="14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B26" s="3">
         <v>105.70027081122315</v>
       </c>
@@ -1057,8 +1236,14 @@
       <c r="I26" s="3">
         <v>155.55125973827421</v>
       </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J26" s="14">
+        <v>22</v>
+      </c>
+      <c r="K26" s="14">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B27" s="2">
         <v>113.91958123550576</v>
       </c>
@@ -1078,8 +1263,14 @@
       <c r="I27" s="2">
         <v>157.25679789397495</v>
       </c>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J27" s="14">
+        <v>23</v>
+      </c>
+      <c r="K27" s="14">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B28" s="3">
         <v>126.08003626488187</v>
       </c>
@@ -1099,8 +1290,14 @@
       <c r="I28" s="3">
         <v>156.41154732853997</v>
       </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J28" s="14">
+        <v>24</v>
+      </c>
+      <c r="K28" s="14">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B29" s="2">
         <v>137.19834965167709</v>
       </c>
@@ -1120,8 +1317,14 @@
       <c r="I29" s="2">
         <v>148.13308971852589</v>
       </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J29" s="14">
+        <v>25</v>
+      </c>
+      <c r="K29" s="14">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B30" s="2">
         <v>229.73562933480542</v>
       </c>
@@ -1141,8 +1344,14 @@
       <c r="I30" s="2">
         <v>70.533761426743652</v>
       </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J30" s="14">
+        <v>26</v>
+      </c>
+      <c r="K30" s="14">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B31" s="2">
         <v>299.1858495324264</v>
       </c>
@@ -1162,8 +1371,14 @@
       <c r="I31" s="2">
         <v>43.5054223994266</v>
       </c>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J31" s="14">
+        <v>27</v>
+      </c>
+      <c r="K31" s="14">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B32" s="3">
         <v>319.57479459972808</v>
       </c>
@@ -1183,8 +1398,14 @@
       <c r="I32" s="3">
         <v>42.021874054685355</v>
       </c>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J32" s="14">
+        <v>28</v>
+      </c>
+      <c r="K32" s="14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B33" s="2">
         <v>323.70190665422706</v>
       </c>
@@ -1204,8 +1425,14 @@
       <c r="I33" s="2">
         <v>54.313728285683382</v>
       </c>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J33" s="14">
+        <v>29</v>
+      </c>
+      <c r="K33" s="14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B34" s="3">
         <v>322.10890627093437</v>
       </c>
@@ -1225,8 +1452,14 @@
       <c r="I34" s="3">
         <v>68.949360083587479</v>
       </c>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J34" s="14">
+        <v>30</v>
+      </c>
+      <c r="K34" s="14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B35" s="2">
         <v>301.44132551238772</v>
       </c>
@@ -1246,8 +1479,14 @@
       <c r="I35" s="2">
         <v>81.061615156702544</v>
       </c>
-    </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J35" s="14">
+        <v>31</v>
+      </c>
+      <c r="K35" s="14">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B36" s="2">
         <v>272.24850416140657</v>
       </c>
@@ -1267,8 +1506,14 @@
       <c r="I36" s="2">
         <v>82.300845323352007</v>
       </c>
-    </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J36" s="14">
+        <v>32</v>
+      </c>
+      <c r="K36" s="14">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B37" s="2">
         <v>246.06771441507522</v>
       </c>
@@ -1288,8 +1533,14 @@
       <c r="I37" s="2">
         <v>91.475432603126748</v>
       </c>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J37" s="14">
+        <v>33</v>
+      </c>
+      <c r="K37" s="14">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B38" s="2">
         <v>147.19879899151798</v>
       </c>
@@ -1309,8 +1560,14 @@
       <c r="I38" s="2">
         <v>165.73755728867269</v>
       </c>
-    </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J38" s="14">
+        <v>34</v>
+      </c>
+      <c r="K38" s="14">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B39" s="3">
         <v>129.97181068433079</v>
       </c>
@@ -1330,8 +1587,14 @@
       <c r="I39" s="3">
         <v>179.72307628748948</v>
       </c>
-    </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J39" s="14">
+        <v>35</v>
+      </c>
+      <c r="K39" s="14">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B40" s="2">
         <v>134.88882465565123</v>
       </c>
@@ -1351,8 +1614,14 @@
       <c r="I40" s="2">
         <v>185.71379416227353</v>
       </c>
-    </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J40" s="14">
+        <v>36</v>
+      </c>
+      <c r="K40" s="14">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B41" s="3">
         <v>147.95449152257351</v>
       </c>
@@ -1372,8 +1641,14 @@
       <c r="I41" s="3">
         <v>187.35112930215965</v>
       </c>
-    </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J41" s="14">
+        <v>37</v>
+      </c>
+      <c r="K41" s="14">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B42" s="2">
         <v>170.57245602710293</v>
       </c>
@@ -1392,6 +1667,12 @@
       </c>
       <c r="I42" s="2">
         <v>176.43021725310777</v>
+      </c>
+      <c r="J42" s="14">
+        <v>38</v>
+      </c>
+      <c r="K42" s="14">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>